<commit_message>
perbaiki dokumen lampiran-lampiran rks
</commit_message>
<xml_diff>
--- a/templates/Lamp 3.xlsx
+++ b/templates/Lamp 3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="45" windowWidth="9690" windowHeight="5985"/>
@@ -157,8 +157,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -207,11 +207,6 @@
       <b/>
       <sz val="10"/>
       <name val="Univers"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Univers"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
@@ -232,6 +227,26 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Univers"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Univers"/>
     </font>
   </fonts>
   <fills count="3">
@@ -398,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -446,7 +461,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -455,7 +470,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -480,14 +495,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -497,6 +508,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,7 +676,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -689,7 +710,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -865,11 +885,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:H6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -903,69 +923,69 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="3:9" ht="15.75">
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="3:9" ht="15.75">
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="3:9" ht="15.75">
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="3:9" ht="14.25">
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="3:9" ht="14.25">
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="3:9" ht="14.25">
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="3:9" ht="15" thickBot="1">
@@ -1424,7 +1444,7 @@
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="36" t="s">
+      <c r="G48" s="48" t="s">
         <v>38</v>
       </c>
       <c r="H48" s="2"/>

</xml_diff>